<commit_message>
to try xml format
</commit_message>
<xml_diff>
--- a/Test Documentation/Checklists/Web_app/Checklists for learn.epam.com _STA course.xlsx
+++ b/Test Documentation/Checklists/Web_app/Checklists for learn.epam.com _STA course.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\Portfolio_Tester\Test Documentation\Checklists\Web_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B80F42-BD30-435D-95A8-16541EA72C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A918A031-71A3-456D-B8A6-B568EBF51B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-4430" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1081,71 +1081,71 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1564,11 +1564,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:P126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1580,7 +1583,7 @@
     <col min="5" max="5" width="12.77734375" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="17" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="78.33203125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="51.77734375" style="28" customWidth="1"/>
     <col min="9" max="9" width="80.5546875" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9.109375" style="2"/>
   </cols>
@@ -1620,16 +1623,16 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="73" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1643,15 +1646,15 @@
       <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1665,8 +1668,8 @@
       <c r="A4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="47" t="s">
@@ -1679,7 +1682,7 @@
       <c r="G4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="71" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1687,8 +1690,8 @@
       <c r="A5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="55"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="48" t="s">
         <v>207</v>
       </c>
@@ -1699,14 +1702,14 @@
       <c r="G5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="59"/>
+      <c r="H5" s="71"/>
     </row>
     <row r="6" spans="1:16" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="55"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="20" t="s">
         <v>215</v>
       </c>
@@ -1725,8 +1728,8 @@
       <c r="A7" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="55"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="48" t="s">
         <v>206</v>
       </c>
@@ -1745,8 +1748,8 @@
       <c r="A8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="55"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="48" t="s">
         <v>201</v>
       </c>
@@ -1757,7 +1760,7 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="59" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1765,8 +1768,8 @@
       <c r="A9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="55"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="48" t="s">
         <v>202</v>
       </c>
@@ -1777,14 +1780,14 @@
       <c r="G9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="71"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="55"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="67"/>
       <c r="D10" s="47" t="s">
         <v>208</v>
       </c>
@@ -1795,7 +1798,7 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1803,15 +1806,15 @@
       <c r="A11" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1821,12 +1824,12 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="54" t="s">
+      <c r="B12" s="70"/>
+      <c r="C12" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="48" t="s">
@@ -1839,16 +1842,16 @@
       <c r="G12" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="71" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="55"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="48" t="s">
         <v>197</v>
       </c>
@@ -1859,14 +1862,14 @@
       <c r="G13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="59"/>
+      <c r="H13" s="71"/>
     </row>
     <row r="14" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="55"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="7" t="s">
         <v>43</v>
       </c>
@@ -1885,8 +1888,8 @@
       <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="55"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="7" t="s">
         <v>45</v>
       </c>
@@ -1905,8 +1908,8 @@
       <c r="A16" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="55"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="48" t="s">
         <v>198</v>
       </c>
@@ -1925,15 +1928,15 @@
       <c r="A17" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1947,8 +1950,8 @@
       <c r="A18" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="54" t="s">
+      <c r="B18" s="75"/>
+      <c r="C18" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="48" t="s">
@@ -1977,8 +1980,8 @@
       <c r="A19" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="55"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="67"/>
       <c r="D19" s="48" t="s">
         <v>204</v>
       </c>
@@ -1997,8 +2000,8 @@
       <c r="A20" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="55"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="48" t="s">
         <v>195</v>
       </c>
@@ -2017,8 +2020,8 @@
       <c r="A21" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="60"/>
-      <c r="C21" s="55"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="67"/>
       <c r="D21" s="48" t="s">
         <v>200</v>
       </c>
@@ -2029,7 +2032,7 @@
       <c r="G21" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="72" t="s">
+      <c r="H21" s="61" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2037,8 +2040,8 @@
       <c r="A22" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="55"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="67"/>
       <c r="D22" s="48" t="s">
         <v>199</v>
       </c>
@@ -2049,14 +2052,14 @@
       <c r="G22" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="73"/>
+      <c r="H22" s="62"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="55"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="67"/>
       <c r="D23" s="48" t="s">
         <v>210</v>
       </c>
@@ -2067,7 +2070,7 @@
       <c r="G23" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="64" t="s">
+      <c r="H23" s="56" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2075,8 +2078,8 @@
       <c r="A24" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="60"/>
-      <c r="C24" s="55"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="48" t="s">
         <v>209</v>
       </c>
@@ -2087,21 +2090,21 @@
       <c r="G24" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="65"/>
+      <c r="H24" s="58"/>
     </row>
     <row r="25" spans="1:16" s="9" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -2111,12 +2114,12 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="56"/>
-      <c r="C26" s="54" t="s">
+      <c r="B26" s="70"/>
+      <c r="C26" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -2129,16 +2132,16 @@
       <c r="G26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="59" t="s">
+      <c r="H26" s="71" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="55"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="67"/>
       <c r="D27" s="48" t="s">
         <v>196</v>
       </c>
@@ -2149,14 +2152,14 @@
       <c r="G27" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="59"/>
+      <c r="H27" s="71"/>
     </row>
     <row r="28" spans="1:16" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="55"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="67"/>
       <c r="D28" s="7" t="s">
         <v>63</v>
       </c>
@@ -2167,7 +2170,7 @@
       <c r="G28" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H28" s="72" t="s">
+      <c r="H28" s="61" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2175,8 +2178,8 @@
       <c r="A29" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="55"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="67"/>
       <c r="D29" s="7" t="s">
         <v>65</v>
       </c>
@@ -2187,14 +2190,14 @@
       <c r="G29" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="74"/>
+      <c r="H29" s="63"/>
     </row>
     <row r="30" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="55"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="67"/>
       <c r="D30" s="48" t="s">
         <v>67</v>
       </c>
@@ -2205,14 +2208,14 @@
       <c r="G30" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H30" s="73"/>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="55"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="67"/>
       <c r="D31" s="48" t="s">
         <v>69</v>
       </c>
@@ -2223,7 +2226,7 @@
       <c r="G31" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="64" t="s">
+      <c r="H31" s="56" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2231,8 +2234,8 @@
       <c r="A32" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="55"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="67"/>
       <c r="D32" s="48" t="s">
         <v>188</v>
       </c>
@@ -2243,14 +2246,14 @@
       <c r="G32" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="65"/>
+      <c r="H32" s="58"/>
     </row>
     <row r="33" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="55"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="67"/>
       <c r="D33" s="7" t="s">
         <v>72</v>
       </c>
@@ -2269,8 +2272,8 @@
       <c r="A34" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="55"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="67"/>
       <c r="D34" s="7" t="s">
         <v>75</v>
       </c>
@@ -2289,15 +2292,15 @@
       <c r="A35" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2311,8 +2314,8 @@
       <c r="A36" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="54" t="s">
+      <c r="B36" s="70"/>
+      <c r="C36" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="47" t="s">
@@ -2325,7 +2328,7 @@
       <c r="G36" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H36" s="59" t="s">
+      <c r="H36" s="71" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2333,8 +2336,8 @@
       <c r="A37" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="55"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="67"/>
       <c r="D37" s="47" t="s">
         <v>81</v>
       </c>
@@ -2345,14 +2348,14 @@
       <c r="G37" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H37" s="59"/>
+      <c r="H37" s="71"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="55"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="67"/>
       <c r="D38" s="47" t="s">
         <v>83</v>
       </c>
@@ -2363,21 +2366,21 @@
       <c r="G38" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H38" s="59"/>
+      <c r="H38" s="71"/>
     </row>
     <row r="39" spans="1:16" s="9" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2391,8 +2394,8 @@
       <c r="A40" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="54" t="s">
+      <c r="B40" s="70"/>
+      <c r="C40" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="47" t="s">
@@ -2413,8 +2416,8 @@
       <c r="A41" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="55"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="67"/>
       <c r="D41" s="47" t="s">
         <v>89</v>
       </c>
@@ -2425,7 +2428,7 @@
       <c r="G41" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H41" s="64" t="s">
+      <c r="H41" s="56" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2433,8 +2436,8 @@
       <c r="A42" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="55"/>
+      <c r="B42" s="70"/>
+      <c r="C42" s="67"/>
       <c r="D42" s="47" t="s">
         <v>91</v>
       </c>
@@ -2445,14 +2448,14 @@
       <c r="G42" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H42" s="65"/>
+      <c r="H42" s="58"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="56"/>
-      <c r="C43" s="55"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="67"/>
       <c r="D43" s="47" t="s">
         <v>189</v>
       </c>
@@ -2463,7 +2466,7 @@
       <c r="G43" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H43" s="64" t="s">
+      <c r="H43" s="56" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2471,8 +2474,8 @@
       <c r="A44" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="56"/>
-      <c r="C44" s="55"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="67"/>
       <c r="D44" s="47" t="s">
         <v>190</v>
       </c>
@@ -2483,14 +2486,14 @@
       <c r="G44" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H44" s="69"/>
+      <c r="H44" s="57"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="56"/>
-      <c r="C45" s="55"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="67"/>
       <c r="D45" s="47" t="s">
         <v>191</v>
       </c>
@@ -2501,14 +2504,14 @@
       <c r="G45" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H45" s="69"/>
+      <c r="H45" s="57"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="56"/>
-      <c r="C46" s="55"/>
+      <c r="B46" s="70"/>
+      <c r="C46" s="67"/>
       <c r="D46" s="47" t="s">
         <v>192</v>
       </c>
@@ -2519,14 +2522,14 @@
       <c r="G46" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="69"/>
+      <c r="H46" s="57"/>
     </row>
     <row r="47" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="56"/>
-      <c r="C47" s="55"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="67"/>
       <c r="D47" s="47" t="s">
         <v>97</v>
       </c>
@@ -2537,21 +2540,21 @@
       <c r="G47" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H47" s="65"/>
+      <c r="H47" s="58"/>
     </row>
     <row r="48" spans="1:16" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -2565,8 +2568,8 @@
       <c r="A49" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="56"/>
-      <c r="C49" s="54" t="s">
+      <c r="B49" s="70"/>
+      <c r="C49" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="48" t="s">
@@ -2579,7 +2582,7 @@
       <c r="G49" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="64" t="s">
+      <c r="H49" s="56" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2587,8 +2590,8 @@
       <c r="A50" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="56"/>
-      <c r="C50" s="55"/>
+      <c r="B50" s="70"/>
+      <c r="C50" s="67"/>
       <c r="D50" s="48" t="s">
         <v>194</v>
       </c>
@@ -2599,14 +2602,14 @@
       <c r="G50" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H50" s="65"/>
+      <c r="H50" s="58"/>
     </row>
     <row r="51" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="56"/>
-      <c r="C51" s="55"/>
+      <c r="B51" s="70"/>
+      <c r="C51" s="67"/>
       <c r="D51" s="7" t="s">
         <v>103</v>
       </c>
@@ -2617,7 +2620,7 @@
       <c r="G51" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H51" s="70" t="s">
+      <c r="H51" s="59" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2625,8 +2628,8 @@
       <c r="A52" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="56"/>
-      <c r="C52" s="55"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="67"/>
       <c r="D52" s="7" t="s">
         <v>105</v>
       </c>
@@ -2637,21 +2640,21 @@
       <c r="G52" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H52" s="71"/>
+      <c r="H52" s="60"/>
     </row>
     <row r="53" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="55"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -2665,8 +2668,8 @@
       <c r="A54" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="56"/>
-      <c r="C54" s="54" t="s">
+      <c r="B54" s="70"/>
+      <c r="C54" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D54" s="7" t="s">
@@ -2679,7 +2682,7 @@
       <c r="G54" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H54" s="70" t="s">
+      <c r="H54" s="59" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2687,8 +2690,8 @@
       <c r="A55" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="56"/>
-      <c r="C55" s="55"/>
+      <c r="B55" s="70"/>
+      <c r="C55" s="67"/>
       <c r="D55" s="7" t="s">
         <v>111</v>
       </c>
@@ -2699,14 +2702,14 @@
       <c r="G55" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H55" s="75"/>
+      <c r="H55" s="64"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="56"/>
-      <c r="C56" s="55"/>
+      <c r="B56" s="70"/>
+      <c r="C56" s="67"/>
       <c r="D56" s="7" t="s">
         <v>113</v>
       </c>
@@ -2717,21 +2720,21 @@
       <c r="G56" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H56" s="71"/>
+      <c r="H56" s="60"/>
     </row>
     <row r="57" spans="1:16" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="58" t="s">
+      <c r="B57" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="55"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -2745,8 +2748,8 @@
       <c r="A58" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="56"/>
-      <c r="C58" s="54" t="s">
+      <c r="B58" s="70"/>
+      <c r="C58" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D58" s="48" t="s">
@@ -2759,7 +2762,7 @@
       <c r="G58" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H58" s="59" t="s">
+      <c r="H58" s="71" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2767,8 +2770,8 @@
       <c r="A59" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="56"/>
-      <c r="C59" s="55"/>
+      <c r="B59" s="70"/>
+      <c r="C59" s="67"/>
       <c r="D59" s="7" t="s">
         <v>118</v>
       </c>
@@ -2779,14 +2782,14 @@
       <c r="G59" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H59" s="62"/>
+      <c r="H59" s="72"/>
     </row>
     <row r="60" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="B60" s="56"/>
-      <c r="C60" s="55"/>
+      <c r="B60" s="70"/>
+      <c r="C60" s="67"/>
       <c r="D60" s="7" t="s">
         <v>120</v>
       </c>
@@ -2797,14 +2800,14 @@
       <c r="G60" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H60" s="62"/>
+      <c r="H60" s="72"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="56"/>
-      <c r="C61" s="55"/>
+      <c r="B61" s="70"/>
+      <c r="C61" s="67"/>
       <c r="D61" s="48" t="s">
         <v>178</v>
       </c>
@@ -2815,19 +2818,19 @@
       <c r="G61" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H61" s="62"/>
+      <c r="H61" s="72"/>
     </row>
     <row r="62" spans="1:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="61" t="s">
+      <c r="A62" s="73" t="s">
         <v>211</v>
       </c>
-      <c r="B62" s="61"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="61"/>
-      <c r="G62" s="61"/>
-      <c r="H62" s="61"/>
+      <c r="B62" s="73"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="73"/>
+      <c r="G62" s="73"/>
+      <c r="H62" s="73"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -2841,15 +2844,15 @@
       <c r="A63" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="58" t="s">
+      <c r="B63" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="58"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
+      <c r="C63" s="55"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="55"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="55"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -2860,11 +2863,11 @@
       <c r="P63" s="2"/>
     </row>
     <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="66" t="s">
+      <c r="A64" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="B64" s="67"/>
-      <c r="C64" s="54" t="s">
+      <c r="B64" s="69"/>
+      <c r="C64" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D64" s="49" t="s">
@@ -2877,14 +2880,14 @@
       <c r="G64" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H64" s="70" t="s">
+      <c r="H64" s="59" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="66"/>
-      <c r="B65" s="67"/>
-      <c r="C65" s="55"/>
+      <c r="A65" s="68"/>
+      <c r="B65" s="69"/>
+      <c r="C65" s="67"/>
       <c r="D65" s="14" t="s">
         <v>126</v>
       </c>
@@ -2895,12 +2898,12 @@
       <c r="G65" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H65" s="75"/>
+      <c r="H65" s="64"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="66"/>
-      <c r="B66" s="67"/>
-      <c r="C66" s="55"/>
+      <c r="A66" s="68"/>
+      <c r="B66" s="69"/>
+      <c r="C66" s="67"/>
       <c r="D66" s="49" t="s">
         <v>185</v>
       </c>
@@ -2911,28 +2914,28 @@
       <c r="G66" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H66" s="71"/>
+      <c r="H66" s="60"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="58" t="s">
+      <c r="B67" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="C67" s="58"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="58"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="58"/>
+      <c r="C67" s="55"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="55"/>
     </row>
     <row r="68" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="56"/>
-      <c r="C68" s="54" t="s">
+      <c r="B68" s="70"/>
+      <c r="C68" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D68" s="48" t="s">
@@ -2945,7 +2948,7 @@
       <c r="G68" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H68" s="64" t="s">
+      <c r="H68" s="56" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2953,8 +2956,8 @@
       <c r="A69" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="56"/>
-      <c r="C69" s="55"/>
+      <c r="B69" s="70"/>
+      <c r="C69" s="67"/>
       <c r="D69" s="7" t="s">
         <v>132</v>
       </c>
@@ -2965,28 +2968,28 @@
       <c r="G69" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H69" s="65"/>
+      <c r="H69" s="58"/>
     </row>
     <row r="70" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="58" t="s">
+      <c r="B70" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="55"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="55"/>
     </row>
     <row r="71" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="56"/>
-      <c r="C71" s="54" t="s">
+      <c r="B71" s="70"/>
+      <c r="C71" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D71" s="7" t="s">
@@ -2999,7 +3002,7 @@
       <c r="G71" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H71" s="59" t="s">
+      <c r="H71" s="71" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3007,8 +3010,8 @@
       <c r="A72" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="B72" s="56"/>
-      <c r="C72" s="55"/>
+      <c r="B72" s="70"/>
+      <c r="C72" s="67"/>
       <c r="D72" s="7" t="s">
         <v>139</v>
       </c>
@@ -3019,14 +3022,14 @@
       <c r="G72" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H72" s="59"/>
+      <c r="H72" s="71"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B73" s="56"/>
-      <c r="C73" s="55"/>
+      <c r="B73" s="70"/>
+      <c r="C73" s="67"/>
       <c r="D73" s="7" t="s">
         <v>141</v>
       </c>
@@ -3037,14 +3040,14 @@
       <c r="G73" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H73" s="59"/>
+      <c r="H73" s="71"/>
     </row>
     <row r="74" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B74" s="56"/>
-      <c r="C74" s="55"/>
+      <c r="B74" s="70"/>
+      <c r="C74" s="67"/>
       <c r="D74" s="7" t="s">
         <v>143</v>
       </c>
@@ -3055,28 +3058,28 @@
       <c r="G74" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H74" s="59"/>
+      <c r="H74" s="71"/>
     </row>
     <row r="75" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B75" s="58" t="s">
+      <c r="B75" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="C75" s="58"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="58"/>
-      <c r="F75" s="58"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="58"/>
+      <c r="C75" s="55"/>
+      <c r="D75" s="55"/>
+      <c r="E75" s="55"/>
+      <c r="F75" s="55"/>
+      <c r="G75" s="55"/>
+      <c r="H75" s="55"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="B76" s="67"/>
-      <c r="C76" s="54" t="s">
+      <c r="B76" s="69"/>
+      <c r="C76" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D76" s="48" t="s">
@@ -3089,7 +3092,7 @@
       <c r="G76" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H76" s="64" t="s">
+      <c r="H76" s="56" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3097,8 +3100,8 @@
       <c r="A77" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="B77" s="67"/>
-      <c r="C77" s="55"/>
+      <c r="B77" s="69"/>
+      <c r="C77" s="67"/>
       <c r="D77" s="48" t="s">
         <v>182</v>
       </c>
@@ -3109,14 +3112,14 @@
       <c r="G77" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H77" s="69"/>
+      <c r="H77" s="57"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="B78" s="67"/>
-      <c r="C78" s="55"/>
+      <c r="B78" s="69"/>
+      <c r="C78" s="67"/>
       <c r="D78" s="7" t="s">
         <v>150</v>
       </c>
@@ -3127,14 +3130,14 @@
       <c r="G78" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H78" s="69"/>
+      <c r="H78" s="57"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="B79" s="67"/>
-      <c r="C79" s="55"/>
+      <c r="B79" s="69"/>
+      <c r="C79" s="67"/>
       <c r="D79" s="7" t="s">
         <v>152</v>
       </c>
@@ -3145,14 +3148,14 @@
       <c r="G79" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H79" s="65"/>
+      <c r="H79" s="58"/>
     </row>
     <row r="80" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="B80" s="67"/>
-      <c r="C80" s="55"/>
+      <c r="B80" s="69"/>
+      <c r="C80" s="67"/>
       <c r="D80" s="7" t="s">
         <v>154</v>
       </c>
@@ -3172,25 +3175,25 @@
       <c r="A81" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="B81" s="58" t="s">
+      <c r="B81" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="C81" s="58"/>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
-      <c r="F81" s="58"/>
-      <c r="G81" s="58"/>
-      <c r="H81" s="58"/>
+      <c r="C81" s="55"/>
+      <c r="D81" s="55"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="55"/>
+      <c r="H81" s="55"/>
       <c r="I81" s="52"/>
     </row>
     <row r="82" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="B82" s="67" t="s">
+      <c r="B82" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="C82" s="54" t="s">
+      <c r="C82" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D82" s="48" t="s">
@@ -3203,7 +3206,7 @@
       <c r="G82" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H82" s="70" t="s">
+      <c r="H82" s="59" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3211,8 +3214,8 @@
       <c r="A83" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="B83" s="67"/>
-      <c r="C83" s="55"/>
+      <c r="B83" s="69"/>
+      <c r="C83" s="67"/>
       <c r="D83" s="7" t="s">
         <v>161</v>
       </c>
@@ -3221,29 +3224,29 @@
       <c r="G83" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H83" s="71"/>
+      <c r="H83" s="60"/>
       <c r="I83" s="11"/>
     </row>
     <row r="84" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="58" t="s">
+      <c r="B84" s="55" t="s">
         <v>163</v>
       </c>
-      <c r="C84" s="58"/>
-      <c r="D84" s="58"/>
-      <c r="E84" s="58"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="58"/>
-      <c r="H84" s="58"/>
+      <c r="C84" s="55"/>
+      <c r="D84" s="55"/>
+      <c r="E84" s="55"/>
+      <c r="F84" s="55"/>
+      <c r="G84" s="55"/>
+      <c r="H84" s="55"/>
     </row>
     <row r="85" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="B85" s="63"/>
-      <c r="C85" s="54" t="s">
+      <c r="B85" s="65"/>
+      <c r="C85" s="66" t="s">
         <v>20</v>
       </c>
       <c r="D85" s="48" t="s">
@@ -3256,7 +3259,7 @@
       <c r="G85" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H85" s="64" t="s">
+      <c r="H85" s="56" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3264,8 +3267,8 @@
       <c r="A86" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="B86" s="63"/>
-      <c r="C86" s="55"/>
+      <c r="B86" s="65"/>
+      <c r="C86" s="67"/>
       <c r="D86" s="48" t="s">
         <v>181</v>
       </c>
@@ -3276,21 +3279,21 @@
       <c r="G86" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H86" s="65"/>
+      <c r="H86" s="58"/>
     </row>
     <row r="87" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B87" s="58" t="s">
+      <c r="B87" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="C87" s="58"/>
-      <c r="D87" s="58"/>
-      <c r="E87" s="58"/>
-      <c r="F87" s="58"/>
-      <c r="G87" s="58"/>
-      <c r="H87" s="58"/>
+      <c r="C87" s="55"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="55"/>
+      <c r="G87" s="55"/>
+      <c r="H87" s="55"/>
     </row>
     <row r="88" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="25" t="s">
@@ -3320,15 +3323,15 @@
       <c r="A89" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="B89" s="58" t="s">
+      <c r="B89" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="C89" s="58"/>
-      <c r="D89" s="58"/>
-      <c r="E89" s="58"/>
-      <c r="F89" s="58"/>
-      <c r="G89" s="58"/>
-      <c r="H89" s="58"/>
+      <c r="C89" s="55"/>
+      <c r="D89" s="55"/>
+      <c r="E89" s="55"/>
+      <c r="F89" s="55"/>
+      <c r="G89" s="55"/>
+      <c r="H89" s="55"/>
     </row>
     <row r="90" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="25" t="s">
@@ -3357,11 +3360,11 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="32"/>
-      <c r="F92" s="68" t="s">
+      <c r="F92" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="G92" s="68"/>
-      <c r="H92" s="68"/>
+      <c r="G92" s="54"/>
+      <c r="H92" s="54"/>
     </row>
     <row r="93" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="32"/>
@@ -3490,6 +3493,62 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="H71:H74"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="H85:H86"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="C68:C69"/>
     <mergeCell ref="F92:H92"/>
     <mergeCell ref="B89:H89"/>
     <mergeCell ref="H43:H47"/>
@@ -3506,63 +3565,8 @@
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="H76:H79"/>
     <mergeCell ref="H82:H83"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="H85:H86"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B81:H81"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:H67"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="H71:H74"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B18:B24"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="3.937007874015748E-2" footer="3.937007874015748E-2"/>
+  <pageSetup paperSize="8" scale="98" fitToHeight="10" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "to try xml format"
This reverts commit f7397ee02c30671e147fd79f6385139e7f14c27c.
</commit_message>
<xml_diff>
--- a/Test Documentation/Checklists/Web_app/Checklists for learn.epam.com _STA course.xlsx
+++ b/Test Documentation/Checklists/Web_app/Checklists for learn.epam.com _STA course.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\Portfolio_Tester\Test Documentation\Checklists\Web_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A918A031-71A3-456D-B8A6-B568EBF51B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B80F42-BD30-435D-95A8-16541EA72C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-4430" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1081,21 +1081,54 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1113,39 +1146,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1564,14 +1564,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:P126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28:H30"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1583,7 +1580,7 @@
     <col min="5" max="5" width="12.77734375" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="17" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="51.77734375" style="28" customWidth="1"/>
+    <col min="8" max="8" width="78.33203125" style="28" customWidth="1"/>
     <col min="9" max="9" width="80.5546875" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9.109375" style="2"/>
   </cols>
@@ -1623,16 +1620,16 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1646,15 +1643,15 @@
       <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1668,8 +1665,8 @@
       <c r="A4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="66" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="47" t="s">
@@ -1682,7 +1679,7 @@
       <c r="G4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="71" t="s">
+      <c r="H4" s="59" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1690,8 +1687,8 @@
       <c r="A5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="67"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="48" t="s">
         <v>207</v>
       </c>
@@ -1702,14 +1699,14 @@
       <c r="G5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="71"/>
+      <c r="H5" s="59"/>
     </row>
     <row r="6" spans="1:16" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="67"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="20" t="s">
         <v>215</v>
       </c>
@@ -1728,8 +1725,8 @@
       <c r="A7" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="67"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="48" t="s">
         <v>206</v>
       </c>
@@ -1748,8 +1745,8 @@
       <c r="A8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="67"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="48" t="s">
         <v>201</v>
       </c>
@@ -1760,7 +1757,7 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="70" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1768,8 +1765,8 @@
       <c r="A9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="67"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="48" t="s">
         <v>202</v>
       </c>
@@ -1780,14 +1777,14 @@
       <c r="G9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="60"/>
+      <c r="H9" s="71"/>
     </row>
     <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="55"/>
       <c r="D10" s="47" t="s">
         <v>208</v>
       </c>
@@ -1798,7 +1795,7 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1806,15 +1803,15 @@
       <c r="A11" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1824,12 +1821,12 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="66" t="s">
+      <c r="B12" s="56"/>
+      <c r="C12" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="48" t="s">
@@ -1842,16 +1839,16 @@
       <c r="G12" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="67"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="48" t="s">
         <v>197</v>
       </c>
@@ -1862,14 +1859,14 @@
       <c r="G13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="71"/>
+      <c r="H13" s="59"/>
     </row>
     <row r="14" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="67"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="7" t="s">
         <v>43</v>
       </c>
@@ -1888,8 +1885,8 @@
       <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="67"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="7" t="s">
         <v>45</v>
       </c>
@@ -1908,8 +1905,8 @@
       <c r="A16" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="67"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="48" t="s">
         <v>198</v>
       </c>
@@ -1928,15 +1925,15 @@
       <c r="A17" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1950,8 +1947,8 @@
       <c r="A18" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="66" t="s">
+      <c r="B18" s="60"/>
+      <c r="C18" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="48" t="s">
@@ -1980,8 +1977,8 @@
       <c r="A19" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="67"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="48" t="s">
         <v>204</v>
       </c>
@@ -2000,8 +1997,8 @@
       <c r="A20" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="75"/>
-      <c r="C20" s="67"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="55"/>
       <c r="D20" s="48" t="s">
         <v>195</v>
       </c>
@@ -2020,8 +2017,8 @@
       <c r="A21" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="67"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="48" t="s">
         <v>200</v>
       </c>
@@ -2032,7 +2029,7 @@
       <c r="G21" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="61" t="s">
+      <c r="H21" s="72" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2040,8 +2037,8 @@
       <c r="A22" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="67"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="55"/>
       <c r="D22" s="48" t="s">
         <v>199</v>
       </c>
@@ -2052,14 +2049,14 @@
       <c r="G22" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="62"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="67"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="55"/>
       <c r="D23" s="48" t="s">
         <v>210</v>
       </c>
@@ -2070,7 +2067,7 @@
       <c r="G23" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="56" t="s">
+      <c r="H23" s="64" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2078,8 +2075,8 @@
       <c r="A24" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="67"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="55"/>
       <c r="D24" s="48" t="s">
         <v>209</v>
       </c>
@@ -2090,21 +2087,21 @@
       <c r="G24" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="58"/>
+      <c r="H24" s="65"/>
     </row>
     <row r="25" spans="1:16" s="9" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -2114,12 +2111,12 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="66" t="s">
+      <c r="B26" s="56"/>
+      <c r="C26" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -2132,16 +2129,16 @@
       <c r="G26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="71" t="s">
+      <c r="H26" s="59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="70"/>
-      <c r="C27" s="67"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="55"/>
       <c r="D27" s="48" t="s">
         <v>196</v>
       </c>
@@ -2152,14 +2149,14 @@
       <c r="G27" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="71"/>
+      <c r="H27" s="59"/>
     </row>
     <row r="28" spans="1:16" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="70"/>
-      <c r="C28" s="67"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="55"/>
       <c r="D28" s="7" t="s">
         <v>63</v>
       </c>
@@ -2170,7 +2167,7 @@
       <c r="G28" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H28" s="61" t="s">
+      <c r="H28" s="72" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2178,8 +2175,8 @@
       <c r="A29" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="67"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="55"/>
       <c r="D29" s="7" t="s">
         <v>65</v>
       </c>
@@ -2190,14 +2187,14 @@
       <c r="G29" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="63"/>
+      <c r="H29" s="74"/>
     </row>
     <row r="30" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="67"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="48" t="s">
         <v>67</v>
       </c>
@@ -2208,14 +2205,14 @@
       <c r="G30" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H30" s="62"/>
+      <c r="H30" s="73"/>
     </row>
     <row r="31" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="67"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="55"/>
       <c r="D31" s="48" t="s">
         <v>69</v>
       </c>
@@ -2226,7 +2223,7 @@
       <c r="G31" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="56" t="s">
+      <c r="H31" s="64" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2234,8 +2231,8 @@
       <c r="A32" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="67"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="55"/>
       <c r="D32" s="48" t="s">
         <v>188</v>
       </c>
@@ -2246,14 +2243,14 @@
       <c r="G32" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="58"/>
+      <c r="H32" s="65"/>
     </row>
     <row r="33" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="70"/>
-      <c r="C33" s="67"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="55"/>
       <c r="D33" s="7" t="s">
         <v>72</v>
       </c>
@@ -2272,8 +2269,8 @@
       <c r="A34" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="70"/>
-      <c r="C34" s="67"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="55"/>
       <c r="D34" s="7" t="s">
         <v>75</v>
       </c>
@@ -2292,15 +2289,15 @@
       <c r="A35" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2314,8 +2311,8 @@
       <c r="A36" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="70"/>
-      <c r="C36" s="66" t="s">
+      <c r="B36" s="56"/>
+      <c r="C36" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="47" t="s">
@@ -2328,7 +2325,7 @@
       <c r="G36" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H36" s="71" t="s">
+      <c r="H36" s="59" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2336,8 +2333,8 @@
       <c r="A37" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="67"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="55"/>
       <c r="D37" s="47" t="s">
         <v>81</v>
       </c>
@@ -2348,14 +2345,14 @@
       <c r="G37" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H37" s="71"/>
+      <c r="H37" s="59"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="67"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="55"/>
       <c r="D38" s="47" t="s">
         <v>83</v>
       </c>
@@ -2366,21 +2363,21 @@
       <c r="G38" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H38" s="71"/>
+      <c r="H38" s="59"/>
     </row>
     <row r="39" spans="1:16" s="9" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="55" t="s">
+      <c r="B39" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2394,8 +2391,8 @@
       <c r="A40" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="70"/>
-      <c r="C40" s="66" t="s">
+      <c r="B40" s="56"/>
+      <c r="C40" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="47" t="s">
@@ -2416,8 +2413,8 @@
       <c r="A41" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="70"/>
-      <c r="C41" s="67"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="55"/>
       <c r="D41" s="47" t="s">
         <v>89</v>
       </c>
@@ -2428,7 +2425,7 @@
       <c r="G41" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H41" s="56" t="s">
+      <c r="H41" s="64" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2436,8 +2433,8 @@
       <c r="A42" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="70"/>
-      <c r="C42" s="67"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="55"/>
       <c r="D42" s="47" t="s">
         <v>91</v>
       </c>
@@ -2448,14 +2445,14 @@
       <c r="G42" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H42" s="58"/>
+      <c r="H42" s="65"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="70"/>
-      <c r="C43" s="67"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="55"/>
       <c r="D43" s="47" t="s">
         <v>189</v>
       </c>
@@ -2466,7 +2463,7 @@
       <c r="G43" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H43" s="56" t="s">
+      <c r="H43" s="64" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2474,8 +2471,8 @@
       <c r="A44" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="70"/>
-      <c r="C44" s="67"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="55"/>
       <c r="D44" s="47" t="s">
         <v>190</v>
       </c>
@@ -2486,14 +2483,14 @@
       <c r="G44" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H44" s="57"/>
+      <c r="H44" s="69"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="70"/>
-      <c r="C45" s="67"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="55"/>
       <c r="D45" s="47" t="s">
         <v>191</v>
       </c>
@@ -2504,14 +2501,14 @@
       <c r="G45" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H45" s="57"/>
+      <c r="H45" s="69"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="70"/>
-      <c r="C46" s="67"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="55"/>
       <c r="D46" s="47" t="s">
         <v>192</v>
       </c>
@@ -2522,14 +2519,14 @@
       <c r="G46" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="57"/>
+      <c r="H46" s="69"/>
     </row>
     <row r="47" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="70"/>
-      <c r="C47" s="67"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="55"/>
       <c r="D47" s="47" t="s">
         <v>97</v>
       </c>
@@ -2540,21 +2537,21 @@
       <c r="G47" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H47" s="58"/>
+      <c r="H47" s="65"/>
     </row>
     <row r="48" spans="1:16" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="55" t="s">
+      <c r="B48" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -2568,8 +2565,8 @@
       <c r="A49" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="70"/>
-      <c r="C49" s="66" t="s">
+      <c r="B49" s="56"/>
+      <c r="C49" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="48" t="s">
@@ -2582,7 +2579,7 @@
       <c r="G49" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="56" t="s">
+      <c r="H49" s="64" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2590,8 +2587,8 @@
       <c r="A50" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="70"/>
-      <c r="C50" s="67"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="55"/>
       <c r="D50" s="48" t="s">
         <v>194</v>
       </c>
@@ -2602,14 +2599,14 @@
       <c r="G50" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H50" s="58"/>
+      <c r="H50" s="65"/>
     </row>
     <row r="51" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="70"/>
-      <c r="C51" s="67"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="55"/>
       <c r="D51" s="7" t="s">
         <v>103</v>
       </c>
@@ -2620,7 +2617,7 @@
       <c r="G51" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H51" s="59" t="s">
+      <c r="H51" s="70" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2628,8 +2625,8 @@
       <c r="A52" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="70"/>
-      <c r="C52" s="67"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="55"/>
       <c r="D52" s="7" t="s">
         <v>105</v>
       </c>
@@ -2640,21 +2637,21 @@
       <c r="G52" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H52" s="60"/>
+      <c r="H52" s="71"/>
     </row>
     <row r="53" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="B53" s="74" t="s">
+      <c r="B53" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="55"/>
-      <c r="H53" s="55"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -2668,8 +2665,8 @@
       <c r="A54" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="70"/>
-      <c r="C54" s="66" t="s">
+      <c r="B54" s="56"/>
+      <c r="C54" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D54" s="7" t="s">
@@ -2682,7 +2679,7 @@
       <c r="G54" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H54" s="59" t="s">
+      <c r="H54" s="70" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2690,8 +2687,8 @@
       <c r="A55" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="70"/>
-      <c r="C55" s="67"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="55"/>
       <c r="D55" s="7" t="s">
         <v>111</v>
       </c>
@@ -2702,14 +2699,14 @@
       <c r="G55" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H55" s="64"/>
+      <c r="H55" s="75"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="70"/>
-      <c r="C56" s="67"/>
+      <c r="B56" s="56"/>
+      <c r="C56" s="55"/>
       <c r="D56" s="7" t="s">
         <v>113</v>
       </c>
@@ -2720,21 +2717,21 @@
       <c r="G56" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H56" s="60"/>
+      <c r="H56" s="71"/>
     </row>
     <row r="57" spans="1:16" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="55" t="s">
+      <c r="B57" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -2748,8 +2745,8 @@
       <c r="A58" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="70"/>
-      <c r="C58" s="66" t="s">
+      <c r="B58" s="56"/>
+      <c r="C58" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D58" s="48" t="s">
@@ -2762,7 +2759,7 @@
       <c r="G58" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H58" s="71" t="s">
+      <c r="H58" s="59" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2770,8 +2767,8 @@
       <c r="A59" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="70"/>
-      <c r="C59" s="67"/>
+      <c r="B59" s="56"/>
+      <c r="C59" s="55"/>
       <c r="D59" s="7" t="s">
         <v>118</v>
       </c>
@@ -2782,14 +2779,14 @@
       <c r="G59" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H59" s="72"/>
+      <c r="H59" s="62"/>
     </row>
     <row r="60" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="B60" s="70"/>
-      <c r="C60" s="67"/>
+      <c r="B60" s="56"/>
+      <c r="C60" s="55"/>
       <c r="D60" s="7" t="s">
         <v>120</v>
       </c>
@@ -2800,14 +2797,14 @@
       <c r="G60" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H60" s="72"/>
+      <c r="H60" s="62"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="70"/>
-      <c r="C61" s="67"/>
+      <c r="B61" s="56"/>
+      <c r="C61" s="55"/>
       <c r="D61" s="48" t="s">
         <v>178</v>
       </c>
@@ -2818,19 +2815,19 @@
       <c r="G61" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H61" s="72"/>
+      <c r="H61" s="62"/>
     </row>
     <row r="62" spans="1:16" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="73" t="s">
+      <c r="A62" s="61" t="s">
         <v>211</v>
       </c>
-      <c r="B62" s="73"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="73"/>
-      <c r="G62" s="73"/>
-      <c r="H62" s="73"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -2844,15 +2841,15 @@
       <c r="A63" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="55" t="s">
+      <c r="B63" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="55"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="55"/>
-      <c r="H63" s="55"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="58"/>
+      <c r="E63" s="58"/>
+      <c r="F63" s="58"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="58"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -2863,11 +2860,11 @@
       <c r="P63" s="2"/>
     </row>
     <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="68" t="s">
+      <c r="A64" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="B64" s="69"/>
-      <c r="C64" s="66" t="s">
+      <c r="B64" s="67"/>
+      <c r="C64" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D64" s="49" t="s">
@@ -2880,14 +2877,14 @@
       <c r="G64" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H64" s="59" t="s">
+      <c r="H64" s="70" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="68"/>
-      <c r="B65" s="69"/>
-      <c r="C65" s="67"/>
+      <c r="A65" s="66"/>
+      <c r="B65" s="67"/>
+      <c r="C65" s="55"/>
       <c r="D65" s="14" t="s">
         <v>126</v>
       </c>
@@ -2898,12 +2895,12 @@
       <c r="G65" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H65" s="64"/>
+      <c r="H65" s="75"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="68"/>
-      <c r="B66" s="69"/>
-      <c r="C66" s="67"/>
+      <c r="A66" s="66"/>
+      <c r="B66" s="67"/>
+      <c r="C66" s="55"/>
       <c r="D66" s="49" t="s">
         <v>185</v>
       </c>
@@ -2914,28 +2911,28 @@
       <c r="G66" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H66" s="60"/>
+      <c r="H66" s="71"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="55" t="s">
+      <c r="B67" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="C67" s="55"/>
-      <c r="D67" s="55"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="55"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="58"/>
+      <c r="E67" s="58"/>
+      <c r="F67" s="58"/>
+      <c r="G67" s="58"/>
+      <c r="H67" s="58"/>
     </row>
     <row r="68" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="70"/>
-      <c r="C68" s="66" t="s">
+      <c r="B68" s="56"/>
+      <c r="C68" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D68" s="48" t="s">
@@ -2948,7 +2945,7 @@
       <c r="G68" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H68" s="56" t="s">
+      <c r="H68" s="64" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2956,8 +2953,8 @@
       <c r="A69" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="70"/>
-      <c r="C69" s="67"/>
+      <c r="B69" s="56"/>
+      <c r="C69" s="55"/>
       <c r="D69" s="7" t="s">
         <v>132</v>
       </c>
@@ -2968,28 +2965,28 @@
       <c r="G69" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H69" s="58"/>
+      <c r="H69" s="65"/>
     </row>
     <row r="70" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="55" t="s">
+      <c r="B70" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="C70" s="55"/>
-      <c r="D70" s="55"/>
-      <c r="E70" s="55"/>
-      <c r="F70" s="55"/>
-      <c r="G70" s="55"/>
-      <c r="H70" s="55"/>
+      <c r="C70" s="58"/>
+      <c r="D70" s="58"/>
+      <c r="E70" s="58"/>
+      <c r="F70" s="58"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="58"/>
     </row>
     <row r="71" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="70"/>
-      <c r="C71" s="66" t="s">
+      <c r="B71" s="56"/>
+      <c r="C71" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D71" s="7" t="s">
@@ -3002,7 +2999,7 @@
       <c r="G71" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H71" s="71" t="s">
+      <c r="H71" s="59" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3010,8 +3007,8 @@
       <c r="A72" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="B72" s="70"/>
-      <c r="C72" s="67"/>
+      <c r="B72" s="56"/>
+      <c r="C72" s="55"/>
       <c r="D72" s="7" t="s">
         <v>139</v>
       </c>
@@ -3022,14 +3019,14 @@
       <c r="G72" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H72" s="71"/>
+      <c r="H72" s="59"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B73" s="70"/>
-      <c r="C73" s="67"/>
+      <c r="B73" s="56"/>
+      <c r="C73" s="55"/>
       <c r="D73" s="7" t="s">
         <v>141</v>
       </c>
@@ -3040,14 +3037,14 @@
       <c r="G73" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H73" s="71"/>
+      <c r="H73" s="59"/>
     </row>
     <row r="74" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B74" s="70"/>
-      <c r="C74" s="67"/>
+      <c r="B74" s="56"/>
+      <c r="C74" s="55"/>
       <c r="D74" s="7" t="s">
         <v>143</v>
       </c>
@@ -3058,28 +3055,28 @@
       <c r="G74" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H74" s="71"/>
+      <c r="H74" s="59"/>
     </row>
     <row r="75" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B75" s="55" t="s">
+      <c r="B75" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="C75" s="55"/>
-      <c r="D75" s="55"/>
-      <c r="E75" s="55"/>
-      <c r="F75" s="55"/>
-      <c r="G75" s="55"/>
-      <c r="H75" s="55"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="58"/>
+      <c r="E75" s="58"/>
+      <c r="F75" s="58"/>
+      <c r="G75" s="58"/>
+      <c r="H75" s="58"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="B76" s="69"/>
-      <c r="C76" s="66" t="s">
+      <c r="B76" s="67"/>
+      <c r="C76" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D76" s="48" t="s">
@@ -3092,7 +3089,7 @@
       <c r="G76" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H76" s="56" t="s">
+      <c r="H76" s="64" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3100,8 +3097,8 @@
       <c r="A77" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="B77" s="69"/>
-      <c r="C77" s="67"/>
+      <c r="B77" s="67"/>
+      <c r="C77" s="55"/>
       <c r="D77" s="48" t="s">
         <v>182</v>
       </c>
@@ -3112,14 +3109,14 @@
       <c r="G77" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H77" s="57"/>
+      <c r="H77" s="69"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="B78" s="69"/>
-      <c r="C78" s="67"/>
+      <c r="B78" s="67"/>
+      <c r="C78" s="55"/>
       <c r="D78" s="7" t="s">
         <v>150</v>
       </c>
@@ -3130,14 +3127,14 @@
       <c r="G78" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H78" s="57"/>
+      <c r="H78" s="69"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="B79" s="69"/>
-      <c r="C79" s="67"/>
+      <c r="B79" s="67"/>
+      <c r="C79" s="55"/>
       <c r="D79" s="7" t="s">
         <v>152</v>
       </c>
@@ -3148,14 +3145,14 @@
       <c r="G79" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H79" s="58"/>
+      <c r="H79" s="65"/>
     </row>
     <row r="80" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="B80" s="69"/>
-      <c r="C80" s="67"/>
+      <c r="B80" s="67"/>
+      <c r="C80" s="55"/>
       <c r="D80" s="7" t="s">
         <v>154</v>
       </c>
@@ -3175,25 +3172,25 @@
       <c r="A81" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="B81" s="55" t="s">
+      <c r="B81" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="C81" s="55"/>
-      <c r="D81" s="55"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55"/>
-      <c r="G81" s="55"/>
-      <c r="H81" s="55"/>
+      <c r="C81" s="58"/>
+      <c r="D81" s="58"/>
+      <c r="E81" s="58"/>
+      <c r="F81" s="58"/>
+      <c r="G81" s="58"/>
+      <c r="H81" s="58"/>
       <c r="I81" s="52"/>
     </row>
     <row r="82" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="B82" s="69" t="s">
+      <c r="B82" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="C82" s="66" t="s">
+      <c r="C82" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D82" s="48" t="s">
@@ -3206,7 +3203,7 @@
       <c r="G82" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H82" s="59" t="s">
+      <c r="H82" s="70" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3214,8 +3211,8 @@
       <c r="A83" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="B83" s="69"/>
-      <c r="C83" s="67"/>
+      <c r="B83" s="67"/>
+      <c r="C83" s="55"/>
       <c r="D83" s="7" t="s">
         <v>161</v>
       </c>
@@ -3224,29 +3221,29 @@
       <c r="G83" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H83" s="60"/>
+      <c r="H83" s="71"/>
       <c r="I83" s="11"/>
     </row>
     <row r="84" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="55" t="s">
+      <c r="B84" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C84" s="55"/>
-      <c r="D84" s="55"/>
-      <c r="E84" s="55"/>
-      <c r="F84" s="55"/>
-      <c r="G84" s="55"/>
-      <c r="H84" s="55"/>
+      <c r="C84" s="58"/>
+      <c r="D84" s="58"/>
+      <c r="E84" s="58"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="58"/>
+      <c r="H84" s="58"/>
     </row>
     <row r="85" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="B85" s="65"/>
-      <c r="C85" s="66" t="s">
+      <c r="B85" s="63"/>
+      <c r="C85" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D85" s="48" t="s">
@@ -3259,7 +3256,7 @@
       <c r="G85" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H85" s="56" t="s">
+      <c r="H85" s="64" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3267,8 +3264,8 @@
       <c r="A86" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="B86" s="65"/>
-      <c r="C86" s="67"/>
+      <c r="B86" s="63"/>
+      <c r="C86" s="55"/>
       <c r="D86" s="48" t="s">
         <v>181</v>
       </c>
@@ -3279,21 +3276,21 @@
       <c r="G86" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H86" s="58"/>
+      <c r="H86" s="65"/>
     </row>
     <row r="87" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B87" s="55" t="s">
+      <c r="B87" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="C87" s="55"/>
-      <c r="D87" s="55"/>
-      <c r="E87" s="55"/>
-      <c r="F87" s="55"/>
-      <c r="G87" s="55"/>
-      <c r="H87" s="55"/>
+      <c r="C87" s="58"/>
+      <c r="D87" s="58"/>
+      <c r="E87" s="58"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="58"/>
+      <c r="H87" s="58"/>
     </row>
     <row r="88" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="25" t="s">
@@ -3323,15 +3320,15 @@
       <c r="A89" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="B89" s="55" t="s">
+      <c r="B89" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="C89" s="55"/>
-      <c r="D89" s="55"/>
-      <c r="E89" s="55"/>
-      <c r="F89" s="55"/>
-      <c r="G89" s="55"/>
-      <c r="H89" s="55"/>
+      <c r="C89" s="58"/>
+      <c r="D89" s="58"/>
+      <c r="E89" s="58"/>
+      <c r="F89" s="58"/>
+      <c r="G89" s="58"/>
+      <c r="H89" s="58"/>
     </row>
     <row r="90" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="25" t="s">
@@ -3360,11 +3357,11 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="32"/>
-      <c r="F92" s="54" t="s">
+      <c r="F92" s="68" t="s">
         <v>173</v>
       </c>
-      <c r="G92" s="54"/>
-      <c r="H92" s="54"/>
+      <c r="G92" s="68"/>
+      <c r="H92" s="68"/>
     </row>
     <row r="93" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="32"/>
@@ -3493,20 +3490,48 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="H43:H47"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="H54:H56"/>
+    <mergeCell ref="H64:H66"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="H76:H79"/>
+    <mergeCell ref="H82:H83"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="H85:H86"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="B54:B56"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="H71:H74"/>
     <mergeCell ref="C12:C16"/>
@@ -3523,50 +3548,21 @@
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B53:H53"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="H85:H86"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B81:H81"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:H67"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="B89:H89"/>
-    <mergeCell ref="H43:H47"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="H54:H56"/>
-    <mergeCell ref="H64:H66"/>
-    <mergeCell ref="H68:H69"/>
-    <mergeCell ref="H76:H79"/>
-    <mergeCell ref="H82:H83"/>
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B18:B24"/>
   </mergeCells>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="3.937007874015748E-2" footer="3.937007874015748E-2"/>
-  <pageSetup paperSize="8" scale="98" fitToHeight="10" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>